<commit_message>
Added Berndorf build icons
</commit_message>
<xml_diff>
--- a/Assets/Excel/Kundendatenbank.xlsx
+++ b/Assets/Excel/Kundendatenbank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\PB Programme\Projekte\TeamProjects ItchIO\Kundendatenbank\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A3E68F-D583-4533-B088-CC62F535F708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06B140C-87A7-4F63-AE69-7243FC05AE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{847D2D25-995A-4D6D-9549-AA573668EDDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{847D2D25-995A-4D6D-9549-AA573668EDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenbank" sheetId="1" r:id="rId1"/>
@@ -330,9 +330,6 @@
     <t>59929 Brilon</t>
   </si>
   <si>
-    <t>Herrn Veile</t>
-  </si>
-  <si>
     <t>Egger Kunststoffe GmbH &amp; Co. KG</t>
   </si>
   <si>
@@ -570,6 +567,9 @@
   </si>
   <si>
     <t>China</t>
+  </si>
+  <si>
+    <t>Veile</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4957CCC-88FC-4002-981F-ECC1B3231AC8}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,22 +1071,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1094,19 +1094,19 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1114,19 +1114,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1294,16 +1294,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>86</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>37</v>
@@ -1314,7 +1314,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>94</v>
@@ -1334,16 +1334,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>37</v>
@@ -1354,7 +1354,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>85</v>
@@ -1374,16 +1374,16 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>37</v>
@@ -1394,16 +1394,16 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>37</v>
@@ -1414,16 +1414,16 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>37</v>
@@ -1454,7 +1454,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>90</v>
@@ -1474,7 +1474,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>90</v>
@@ -1500,10 +1500,10 @@
         <v>43</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>37</v>
@@ -1514,16 +1514,16 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>37</v>
@@ -1614,39 +1614,39 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1654,19 +1654,19 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1714,16 +1714,16 @@
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>50</v>
@@ -1734,10 +1734,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>50</v>
@@ -1794,13 +1794,13 @@
         <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>58</v>
@@ -1894,19 +1894,19 @@
         <v>23</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,39 +1914,39 @@
         <v>20</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2011,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2019,7 +2019,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -2027,7 +2027,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -2035,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -2051,7 +2051,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -2115,12 +2115,12 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" t="s">
         <v>35</v>
@@ -2131,7 +2131,7 @@
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -2184,12 +2184,12 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>